<commit_message>
Paleta Esteban y arreglados algunos materiales
</commit_message>
<xml_diff>
--- a/PACMA/Assets/Textos/mat.xlsx
+++ b/PACMA/Assets/Textos/mat.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\Documents\GitHub\PACMA\PACMA\Assets\Textos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386A8F76-1A33-46E2-9F1A-2121ABE25637}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6384"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Material</t>
   </si>
@@ -114,12 +115,27 @@
   </si>
   <si>
     <t>Asientos</t>
+  </si>
+  <si>
+    <t>Gata</t>
+  </si>
+  <si>
+    <t>Gatos</t>
+  </si>
+  <si>
+    <t>Conductor</t>
+  </si>
+  <si>
+    <t>Copiloto</t>
+  </si>
+  <si>
+    <t>Falda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,9 +209,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -219,6 +232,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,260 +514,292 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="6" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="6" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+      <c r="F17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>